<commit_message>
last changes before weekend
</commit_message>
<xml_diff>
--- a/test cases/case_A_2.xlsx
+++ b/test cases/case_A_2.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Projekte\GitHub\iDesignRES_transcompmodel\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA80B13-7479-42E0-8232-1934227E9DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A87DC2-6E86-4B11-A749-31887A01F7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16164" yWindow="348" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="modelrun_setting" sheetId="2" r:id="rId1"/>
+    <sheet name="set_nb_names" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,17 +26,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Region</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>set_type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_activated </t>
+  </si>
+  <si>
+    <t>explanatory_comment</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>regional</t>
+  </si>
+  <si>
+    <t>interregional</t>
+  </si>
+  <si>
+    <t>vehicle stock</t>
+  </si>
+  <si>
+    <t>mode infrastructure</t>
+  </si>
+  <si>
+    <t>fueling infrastructure</t>
+  </si>
+  <si>
+    <t>fuel supply infrastructure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +123,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,31 +405,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F84D93-845F-4D6B-A86F-EE740651BA3A}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="b">
         <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F84D93-845F-4D6B-A86F-EE740651BA3A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>